<commit_message>
Working on dec. nepr from Al
</commit_message>
<xml_diff>
--- a/Bundle/Destination.xlsx
+++ b/Bundle/Destination.xlsx
@@ -454,7 +454,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>C:/Red-Nord/DISC T/REGISTRU AUTORIZATII</t>
+          <t>D:/Red-Nord/DISC T/REGISTRU AUTORIZATII</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:/Red-Nord/DISC T/DECONECTARI ZILNICE</t>
+          <t>D:/Red-Nord/DISC T/DECONECTARI ZILNICE</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Red-Nord/DISC T/RAPORT PDJT</t>
+          <t>D:/Red-Nord/DISC T/RAPORT PDJT</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,11 @@
           <t>Destinatie ANALIZA ANUALA</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D:/Red-Nord/DISC T/Analiza</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>